<commit_message>
Add ISO date converter
</commit_message>
<xml_diff>
--- a/test_data/simple01.xlsx
+++ b/test_data/simple01.xlsx
@@ -73,12 +73,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="168" formatCode="0.00%"/>
+    <numFmt numFmtId="169" formatCode="DD/MM/YY\ HH:MM"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -145,7 +146,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -167,6 +168,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -193,9 +198,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>731520</xdr:colOff>
+      <xdr:colOff>731160</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -209,7 +214,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="39600" y="2391120"/>
-          <a:ext cx="2317320" cy="2235240"/>
+          <a:ext cx="2316960" cy="2234880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -235,9 +240,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>157320</xdr:colOff>
+      <xdr:colOff>156960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -251,7 +256,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="360" y="401040"/>
-          <a:ext cx="6659280" cy="6424200"/>
+          <a:ext cx="6658920" cy="6423840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -274,12 +279,14 @@
   <dimension ref="B2:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,7 +391,7 @@
         <f aca="false">10/3</f>
         <v>3.33333333333333</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="e">

</xml_diff>

<commit_message>
Add --no-prefix option - switch to SuperCSV to resolve quoting https://stackoverflow.com/questions/60906988/java-commons-csv-quotemode-minimal-quotes-too-much
</commit_message>
<xml_diff>
--- a/test_data/simple01.xlsx
+++ b/test_data/simple01.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t xml:space="preserve">col1</t>
   </si>
@@ -36,25 +36,28 @@
     <t xml:space="preserve">col4</t>
   </si>
   <si>
+    <t xml:space="preserve">A B    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOO "0"</t>
+  </si>
+  <si>
     <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FOO "0"</t>
   </si>
   <si>
     <t xml:space="preserve">#HERE!</t>
@@ -198,9 +201,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>731160</xdr:colOff>
+      <xdr:colOff>730800</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>74520</xdr:rowOff>
+      <xdr:rowOff>74160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -214,7 +217,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="39600" y="2391120"/>
-          <a:ext cx="2316960" cy="2234880"/>
+          <a:ext cx="2316600" cy="2234520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -240,9 +243,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>156960</xdr:colOff>
+      <xdr:colOff>156600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -256,7 +259,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="360" y="401040"/>
-          <a:ext cx="6658920" cy="6423840"/>
+          <a:ext cx="6658560" cy="6423480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -279,7 +282,7 @@
   <dimension ref="B2:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -367,13 +370,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>4</v>
       </c>
       <c r="G8" s="5" t="n">
         <v>0.1234</v>
@@ -399,7 +402,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -438,10 +441,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -449,7 +452,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>5</v>
@@ -471,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>9</v>

</xml_diff>